<commit_message>
update sim idea table
</commit_message>
<xml_diff>
--- a/SIMULATION_POLIGON/simulation_ideas_table.xlsx
+++ b/SIMULATION_POLIGON/simulation_ideas_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Qba Liu\Documents\STUDIA\BIOINF_MASTER_BERLIN\MASTER_THESIS\SIMULATION_POLIGON\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6022387F-3116-4482-BB58-480FCDDE5B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF52D68-9043-442E-8733-CB8DBDF92A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{CC93E554-30B0-490D-8CFE-132AEC6C27E9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="28">
   <si>
     <t>description</t>
   </si>
@@ -86,6 +86,169 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t xml:space="preserve">level1: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">covariance structure; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>level2:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> effect size;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> level3:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sample size</t>
+    </r>
+  </si>
+  <si>
+    <t>correlation</t>
+  </si>
+  <si>
+    <t>variance</t>
+  </si>
+  <si>
+    <t>mu0</t>
+  </si>
+  <si>
+    <t>location of mu0</t>
+  </si>
+  <si>
+    <t>effect direction</t>
+  </si>
+  <si>
+    <t>n_iter maxtest</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>n_iter_max_test</t>
+  </si>
+  <si>
+    <t>n_iter_maxtest</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>level1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: sample size; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>level2:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> effect size; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>level3:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> n_iter_maxtest</t>
+    </r>
+  </si>
+  <si>
+    <t>In this simulation I just want to test how much iterations of the maximum test do we need to get an acceptable power with the given sample size and the given effect size.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>level1:</t>
     </r>
     <r>
@@ -117,7 +280,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> dimensionality; </t>
+      <t xml:space="preserve"> effect size; </t>
     </r>
     <r>
       <rPr>
@@ -138,171 +301,11 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> effect size</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">level1: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">covariance structure; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>level2:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> effect size;</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> level3:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> sample size</t>
-    </r>
-  </si>
-  <si>
-    <t>correlation</t>
-  </si>
-  <si>
-    <t>variance</t>
-  </si>
-  <si>
-    <t>mu0</t>
-  </si>
-  <si>
-    <t>location of mu0</t>
-  </si>
-  <si>
-    <t>effect direction</t>
-  </si>
-  <si>
-    <t>n_iter maxtest</t>
-  </si>
-  <si>
-    <t>alpha</t>
-  </si>
-  <si>
-    <t>n_iter_max_test</t>
-  </si>
-  <si>
-    <t>n_iter_maxtest</t>
-  </si>
-  <si>
-    <t>comment</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>level1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: sample size; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>level2:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> effect size; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>level3:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> n_iter_maxtest</t>
-    </r>
-  </si>
-  <si>
-    <t>In this simulation I just want to test how much iterations of the maximum test do we need to get an acceptable power with the given sample size and the given effect size.</t>
+      <t xml:space="preserve"> dimensionality</t>
+    </r>
+  </si>
+  <si>
+    <t>THE COMBNINATION OF EFFECT SIZE AND ALTERNATIVE PATTERN DOES NOT MAKE SENSE</t>
   </si>
 </sst>
 </file>
@@ -464,12 +467,42 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -478,36 +511,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -843,10 +846,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E7E069-D7D9-4B6C-8EEC-D70EFC6B3529}">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="B26" workbookViewId="0">
+      <selection activeCell="E34" sqref="E33:E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -901,40 +904,40 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="42" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>3</v>
       </c>
@@ -948,11 +951,11 @@
         <v>0</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="9">
+      <c r="A22" s="20">
         <v>1</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -961,107 +964,107 @@
       <c r="C22" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="10"/>
+      <c r="D22" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="13"/>
     </row>
     <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="9"/>
+      <c r="A23" s="20"/>
       <c r="B23" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="9"/>
+      <c r="A24" s="20"/>
       <c r="B24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="9"/>
+      <c r="A25" s="20"/>
       <c r="B25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="20"/>
+      <c r="B26" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="9"/>
-      <c r="B26" s="4" t="s">
+      <c r="C26" s="4"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="20"/>
+      <c r="B27" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="9"/>
-      <c r="B27" s="4" t="s">
+      <c r="C27" s="4"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="20"/>
+      <c r="B28" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="20"/>
+      <c r="B29" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="4"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="20"/>
+      <c r="B30" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="20"/>
+      <c r="B31" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="9"/>
-      <c r="B28" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="9"/>
-      <c r="B29" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="9"/>
-      <c r="B30" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="9"/>
-      <c r="B31" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="C31" s="4"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="9"/>
+      <c r="A32" s="20"/>
       <c r="B32" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C32" s="4"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="11">
+      <c r="A33" s="21">
         <v>2</v>
       </c>
       <c r="B33" s="7" t="s">
@@ -1070,262 +1073,204 @@
       <c r="C33" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D33" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E33" s="14"/>
+      <c r="D33" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" s="9"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="12"/>
-      <c r="B34" s="7" t="s">
+      <c r="A34" s="22"/>
+      <c r="B34" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="7"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+    </row>
+    <row r="35" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="22"/>
+      <c r="B35" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="7"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="22"/>
+      <c r="B36" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="7"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" s="23"/>
+      <c r="B37" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="7"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="14">
+        <v>3</v>
+      </c>
+      <c r="B38" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C38" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" s="15"/>
+      <c r="B39" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="15"/>
+      <c r="E39" s="18"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" s="15"/>
+      <c r="B40" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" s="15"/>
+      <c r="E40" s="18"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="15"/>
+      <c r="B41" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="12"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="18"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" s="15"/>
+      <c r="B42" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="12"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="18"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" s="15"/>
+      <c r="B43" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="12"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="18"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" s="15"/>
+      <c r="B44" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" s="12"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="18"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" s="15"/>
+      <c r="B45" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" s="12"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="18"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" s="15"/>
+      <c r="B46" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C46" s="12"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="18"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" s="15"/>
+      <c r="B47" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47" s="12"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="18"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" s="16"/>
+      <c r="B48" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-    </row>
-    <row r="35" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A35" s="12"/>
-      <c r="B35" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="12"/>
-      <c r="B36" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="12"/>
-      <c r="B37" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="7"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="12"/>
-      <c r="B38" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C38" s="7"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="12"/>
-      <c r="B39" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C39" s="7"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="15"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="12"/>
-      <c r="B40" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C40" s="7"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="12"/>
-      <c r="B41" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C41" s="7"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="12"/>
-      <c r="B42" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C42" s="7"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="15"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="13"/>
-      <c r="B43" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C43" s="7"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" s="17">
-        <v>3</v>
-      </c>
-      <c r="B44" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C44" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D44" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E44" s="21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="19"/>
-      <c r="B45" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C45" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" s="19"/>
-      <c r="E45" s="22"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="19"/>
-      <c r="B46" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C46" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D46" s="19"/>
-      <c r="E46" s="22"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="19"/>
-      <c r="B47" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C47" s="18"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="22"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="19"/>
-      <c r="B48" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C48" s="18"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="22"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="19"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" s="19"/>
-      <c r="B49" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C49" s="18"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="22"/>
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="19"/>
-      <c r="B50" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C50" s="18"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="22"/>
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51" s="19"/>
-      <c r="B51" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C51" s="18"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="22"/>
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52" s="19"/>
-      <c r="B52" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C52" s="18"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="22"/>
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A53" s="19"/>
-      <c r="B53" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C53" s="18"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="22"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="20"/>
-      <c r="B54" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C54" s="18"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="23"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56" s="3"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" s="3"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58" s="3"/>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A59" s="3"/>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="7">
     <mergeCell ref="E22:E32"/>
-    <mergeCell ref="E33:E43"/>
-    <mergeCell ref="A44:A54"/>
-    <mergeCell ref="D44:D54"/>
-    <mergeCell ref="E44:E54"/>
+    <mergeCell ref="A38:A48"/>
+    <mergeCell ref="D38:D48"/>
+    <mergeCell ref="E38:E48"/>
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="D22:D32"/>
-    <mergeCell ref="A33:A43"/>
-    <mergeCell ref="D33:D43"/>
+    <mergeCell ref="A33:A37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add sim2 and vis of sim1 res
</commit_message>
<xml_diff>
--- a/SIMULATION_POLIGON/simulation_ideas_table.xlsx
+++ b/SIMULATION_POLIGON/simulation_ideas_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Qba Liu\Documents\STUDIA\BIOINF_MASTER_BERLIN\MASTER_THESIS\SIMULATION_POLIGON\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF52D68-9043-442E-8733-CB8DBDF92A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF03B561-22B4-463A-8F48-6947DFDEDB44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{CC93E554-30B0-490D-8CFE-132AEC6C27E9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
   <si>
     <t>description</t>
   </si>
@@ -280,32 +280,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> effect size; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>level3:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> dimensionality</t>
-    </r>
-  </si>
-  <si>
-    <t>THE COMBNINATION OF EFFECT SIZE AND ALTERNATIVE PATTERN DOES NOT MAKE SENSE</t>
+      <t xml:space="preserve"> sample size</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -846,10 +822,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E7E069-D7D9-4B6C-8EEC-D70EFC6B3529}">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B26" workbookViewId="0">
-      <selection activeCell="E34" sqref="E33:E34"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1083,74 +1059,72 @@
       <c r="B34" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="7"/>
+      <c r="C34" s="7" t="s">
+        <v>4</v>
+      </c>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
     </row>
-    <row r="35" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="22"/>
       <c r="B35" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="10"/>
-      <c r="E35" s="10" t="s">
-        <v>27</v>
-      </c>
+      <c r="E35" s="10"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="22"/>
       <c r="B36" s="7" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="23"/>
+      <c r="A37" s="22"/>
       <c r="B37" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" s="7"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="23"/>
+      <c r="B38" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="7"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="14">
+      <c r="C38" s="7"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" s="14">
         <v>3</v>
       </c>
-      <c r="B38" s="12" t="s">
+      <c r="B39" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C39" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="14" t="s">
+      <c r="D39" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E38" s="17" t="s">
+      <c r="E39" s="17" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="15"/>
-      <c r="B39" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="15"/>
-      <c r="E39" s="18"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="15"/>
       <c r="B40" s="12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D40" s="15"/>
       <c r="E40" s="18"/>
@@ -1158,16 +1132,18 @@
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="15"/>
       <c r="B41" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>22</v>
+      </c>
       <c r="D41" s="15"/>
       <c r="E41" s="18"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="15"/>
       <c r="B42" s="12" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C42" s="12"/>
       <c r="D42" s="15"/>
@@ -1176,7 +1152,7 @@
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="15"/>
       <c r="B43" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C43" s="12"/>
       <c r="D43" s="15"/>
@@ -1185,7 +1161,7 @@
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="15"/>
       <c r="B44" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C44" s="12"/>
       <c r="D44" s="15"/>
@@ -1194,7 +1170,7 @@
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="15"/>
       <c r="B45" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C45" s="12"/>
       <c r="D45" s="15"/>
@@ -1203,7 +1179,7 @@
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="15"/>
       <c r="B46" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C46" s="12"/>
       <c r="D46" s="15"/>
@@ -1212,27 +1188,29 @@
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="15"/>
       <c r="B47" s="12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C47" s="12"/>
       <c r="D47" s="15"/>
       <c r="E47" s="18"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="16"/>
+      <c r="A48" s="15"/>
       <c r="B48" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C48" s="12"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="18"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" s="16"/>
+      <c r="B49" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C48" s="12"/>
-      <c r="D48" s="16"/>
-      <c r="E48" s="19"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="19"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="3"/>
@@ -1262,15 +1240,22 @@
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
     </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" s="3"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="E22:E32"/>
-    <mergeCell ref="A38:A48"/>
-    <mergeCell ref="D38:D48"/>
-    <mergeCell ref="E38:E48"/>
+    <mergeCell ref="A39:A49"/>
+    <mergeCell ref="D39:D49"/>
+    <mergeCell ref="E39:E49"/>
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="D22:D32"/>
-    <mergeCell ref="A33:A37"/>
+    <mergeCell ref="A33:A38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update ideas table and add zipped sim2 output
</commit_message>
<xml_diff>
--- a/SIMULATION_POLIGON/simulation_ideas_table.xlsx
+++ b/SIMULATION_POLIGON/simulation_ideas_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Qba Liu\Documents\STUDIA\BIOINF_MASTER_BERLIN\MASTER_THESIS\SIMULATION_POLIGON\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF03B561-22B4-463A-8F48-6947DFDEDB44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2892ABC-EE4E-4073-8DDC-DC89333A5E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{CC93E554-30B0-490D-8CFE-132AEC6C27E9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="27">
   <si>
     <t>description</t>
   </si>
@@ -172,6 +172,9 @@
     <t>comment</t>
   </si>
   <si>
+    <t>In this simulation I just want to test how much iterations of the maximum test do we need to get an acceptable power with the given sample size and the given effect size.</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -181,7 +184,51 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>level1</t>
+      <t>level1:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> alternative pattern; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>level2:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sample size</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>level0: covariance structures; level1</t>
     </r>
     <r>
       <rPr>
@@ -234,53 +281,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> n_iter_maxtest</t>
-    </r>
-  </si>
-  <si>
-    <t>In this simulation I just want to test how much iterations of the maximum test do we need to get an acceptable power with the given sample size and the given effect size.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>level1:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> alternative pattern; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>level2:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> sample size</t>
     </r>
   </si>
 </sst>
@@ -288,7 +288,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,6 +316,12 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -417,7 +423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -486,6 +492,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -824,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E7E069-D7D9-4B6C-8EEC-D70EFC6B3529}">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B26" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="B32" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39:D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1050,7 +1059,7 @@
         <v>10</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E33" s="9"/>
     </row>
@@ -1112,10 +1121,10 @@
         <v>4</v>
       </c>
       <c r="D39" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E39" s="17" t="s">
         <v>24</v>
-      </c>
-      <c r="E39" s="17" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
@@ -1131,9 +1140,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="15"/>
-      <c r="B41" s="12" t="s">
-        <v>10</v>
-      </c>
+      <c r="B41" s="12"/>
       <c r="C41" s="12" t="s">
         <v>22</v>
       </c>
@@ -1142,10 +1149,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="15"/>
-      <c r="B42" s="12" t="s">
+      <c r="B42" s="24"/>
+      <c r="C42" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="12"/>
       <c r="D42" s="15"/>
       <c r="E42" s="18"/>
     </row>

</xml_diff>

<commit_message>
add new sim idea
</commit_message>
<xml_diff>
--- a/SIMULATION_POLIGON/simulation_ideas_table.xlsx
+++ b/SIMULATION_POLIGON/simulation_ideas_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Qba Liu\Documents\STUDIA\BIOINF_MASTER_BERLIN\MASTER_THESIS\SIMULATION_POLIGON\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C69BDBE-A5B3-4D28-8E23-55B7BC588C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DED92D8-B095-4042-A31B-B2FC9DECBB3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{CC93E554-30B0-490D-8CFE-132AEC6C27E9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="32">
   <si>
     <t>description</t>
   </si>
@@ -296,9 +296,6 @@
     </r>
   </si>
   <si>
-    <t>effect dize</t>
-  </si>
-  <si>
     <t>aleternative pattern</t>
   </si>
   <si>
@@ -457,6 +454,77 @@
   </si>
   <si>
     <t>In this simulation I just want to see if there variance and the correlation have an effect on the power for different combinations of the covariance structure, sample size and dimensionality.</t>
+  </si>
+  <si>
+    <t>alpga</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>level1:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  covariance structure;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> level2:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> columns under effect; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">level3: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sample size</t>
+    </r>
+  </si>
+  <si>
+    <t>Here I just want to look at how the number of columns under effect influences the power across different covariance structures and sample sizes</t>
   </si>
 </sst>
 </file>
@@ -494,7 +562,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -522,6 +590,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -590,7 +664,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -625,46 +699,67 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1001,10 +1096,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E7E069-D7D9-4B6C-8EEC-D70EFC6B3529}">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="C50" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1035,7 +1130,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="19">
+      <c r="A2" s="25">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1044,107 +1139,107 @@
       <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="12"/>
+      <c r="E2" s="24"/>
     </row>
     <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="19"/>
+      <c r="A3" s="25"/>
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="19"/>
+      <c r="A4" s="25"/>
       <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="19"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="19"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="19"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="19"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="19"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="19"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="19"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="3"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="19"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="3"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="20">
+      <c r="A13" s="12">
         <v>2</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -1159,7 +1254,7 @@
       <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="21"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="6" t="s">
         <v>18</v>
       </c>
@@ -1170,378 +1265,519 @@
       <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="21"/>
-      <c r="B15" s="5" t="s">
-        <v>14</v>
+      <c r="A15" s="13"/>
+      <c r="B15" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="21"/>
-      <c r="B16" s="5" t="s">
-        <v>9</v>
+      <c r="A16" s="13"/>
+      <c r="B16" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="21"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="22"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="5" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C18" s="5"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="13">
-        <v>3</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="16"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="14"/>
-      <c r="B20" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="14"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10" t="s">
+      <c r="B21" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="18">
+        <v>3</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="21"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="19"/>
+      <c r="B23" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="19"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="14"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="10" t="s">
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="19"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="14"/>
-      <c r="B23" s="10" t="s">
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="19"/>
+      <c r="B26" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="14"/>
-      <c r="B24" s="10" t="s">
+      <c r="C26" s="10"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="19"/>
+      <c r="B27" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="14"/>
-      <c r="B25" s="10" t="s">
+      <c r="C27" s="10"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="19"/>
+      <c r="B28" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="14"/>
-      <c r="B26" s="10" t="s">
+      <c r="C28" s="10"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="19"/>
+      <c r="B29" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="10"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="14"/>
-      <c r="B27" s="10" t="s">
+      <c r="C29" s="10"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="19"/>
+      <c r="B30" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="14"/>
-      <c r="B28" s="10" t="s">
+      <c r="C30" s="10"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="19"/>
+      <c r="B31" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="10"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="15"/>
-      <c r="B29" s="10" t="s">
+      <c r="C31" s="10"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="20"/>
+      <c r="B32" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="10"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="20">
+      <c r="C32" s="10"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="12">
         <v>4</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B33" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C33" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="23" t="s">
+      <c r="D33" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E33" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="23" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="21"/>
-      <c r="B31" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C31" s="5" t="s">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="13"/>
+      <c r="B34" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="21"/>
-      <c r="B32" s="5" t="s">
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" s="13"/>
+      <c r="B35" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="21"/>
-      <c r="B33" s="5" t="s">
+      <c r="C35" s="5"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="13"/>
+      <c r="B36" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="21"/>
-      <c r="B34" s="5" t="s">
+      <c r="C36" s="5"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" s="13"/>
+      <c r="B37" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="5"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="21"/>
-      <c r="B35" s="5" t="s">
+      <c r="C37" s="5"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="13"/>
+      <c r="B38" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="21"/>
-      <c r="B36" s="5" t="s">
+      <c r="C38" s="5"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" s="13"/>
+      <c r="B39" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="21"/>
-      <c r="B37" s="5" t="s">
+      <c r="C39" s="5"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" s="13"/>
+      <c r="B40" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="21"/>
-      <c r="B38" s="5" t="s">
+      <c r="C40" s="5"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="13"/>
+      <c r="B41" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="24"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="21"/>
-      <c r="B39" s="5" t="s">
+      <c r="C41" s="5"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" s="13"/>
+      <c r="B42" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C39" s="5"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="21"/>
-      <c r="B40" s="5" t="s">
+      <c r="C42" s="5"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" s="13"/>
+      <c r="B43" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="5"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="24"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="22"/>
-      <c r="B41" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C41" s="5"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="13">
-        <v>5</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D42" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E42" s="16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="14"/>
-      <c r="B43" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D43" s="17"/>
-      <c r="E43" s="17"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="14"/>
-      <c r="B44" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>14</v>
-      </c>
+      <c r="B44" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" s="5"/>
       <c r="D44" s="17"/>
       <c r="E44" s="17"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="14"/>
+      <c r="A45" s="18">
+        <v>5</v>
+      </c>
       <c r="B45" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E45" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" s="19"/>
+      <c r="B46" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46" s="22"/>
+      <c r="E46" s="22"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" s="19"/>
+      <c r="B47" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" s="22"/>
+      <c r="E47" s="22"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" s="19"/>
+      <c r="B48" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="C48" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D45" s="17"/>
-      <c r="E45" s="17"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="14"/>
-      <c r="B46" s="10" t="s">
+      <c r="D48" s="22"/>
+      <c r="E48" s="22"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" s="19"/>
+      <c r="B49" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="C49" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="14"/>
-      <c r="B47" s="10" t="s">
+      <c r="D49" s="22"/>
+      <c r="E49" s="22"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" s="19"/>
+      <c r="B50" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C47" s="10"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="17"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="14"/>
-      <c r="B48" s="10" t="s">
+      <c r="C50" s="10"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="22"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" s="19"/>
+      <c r="B51" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C48" s="10"/>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" s="14"/>
-      <c r="B49" s="10" t="s">
+      <c r="C51" s="10"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="22"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" s="19"/>
+      <c r="B52" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C49" s="10"/>
-      <c r="D49" s="17"/>
-      <c r="E49" s="17"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="15"/>
-      <c r="B50" s="10" t="s">
+      <c r="C52" s="10"/>
+      <c r="D52" s="22"/>
+      <c r="E52" s="22"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" s="19"/>
+      <c r="B53" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53" s="10"/>
+      <c r="D53" s="22"/>
+      <c r="E53" s="22"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" s="20"/>
+      <c r="B54" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C50" s="10"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="23"/>
+      <c r="E54" s="23"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" s="26">
+        <v>6</v>
+      </c>
+      <c r="B55" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="E55" s="28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56" s="29"/>
+      <c r="B56" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" s="30"/>
+      <c r="E56" s="30"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" s="29"/>
+      <c r="B57" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C57" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57" s="30"/>
+      <c r="E57" s="30"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58" s="29"/>
+      <c r="B58" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C58" s="27"/>
+      <c r="D58" s="30"/>
+      <c r="E58" s="30"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59" s="29"/>
+      <c r="B59" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C59" s="27"/>
+      <c r="D59" s="30"/>
+      <c r="E59" s="30"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60" s="29"/>
+      <c r="B60" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C60" s="27"/>
+      <c r="D60" s="30"/>
+      <c r="E60" s="30"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61" s="29"/>
+      <c r="B61" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" s="27"/>
+      <c r="D61" s="30"/>
+      <c r="E61" s="30"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A62" s="29"/>
+      <c r="B62" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" s="27"/>
+      <c r="D62" s="30"/>
+      <c r="E62" s="30"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A63" s="29"/>
+      <c r="B63" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C63" s="27"/>
+      <c r="D63" s="30"/>
+      <c r="E63" s="30"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A64" s="31"/>
+      <c r="B64" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C64" s="27"/>
+      <c r="D64" s="32"/>
+      <c r="E64" s="32"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A30:A41"/>
-    <mergeCell ref="D30:D41"/>
-    <mergeCell ref="E30:E41"/>
-    <mergeCell ref="A42:A50"/>
-    <mergeCell ref="D42:D50"/>
-    <mergeCell ref="E42:E50"/>
+  <mergeCells count="16">
+    <mergeCell ref="A55:A64"/>
+    <mergeCell ref="D55:D64"/>
+    <mergeCell ref="E55:E64"/>
     <mergeCell ref="E2:E12"/>
-    <mergeCell ref="A19:A29"/>
-    <mergeCell ref="D19:D29"/>
-    <mergeCell ref="E19:E29"/>
+    <mergeCell ref="A22:A32"/>
+    <mergeCell ref="D22:D32"/>
+    <mergeCell ref="E22:E32"/>
     <mergeCell ref="A2:A12"/>
     <mergeCell ref="D2:D12"/>
-    <mergeCell ref="A13:A18"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="A33:A44"/>
+    <mergeCell ref="D33:D44"/>
+    <mergeCell ref="E33:E44"/>
+    <mergeCell ref="A45:A54"/>
+    <mergeCell ref="D45:D54"/>
+    <mergeCell ref="E45:E54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>